<commit_message>
Making the % hit vs. charge correlation graphs easier to read.
</commit_message>
<xml_diff>
--- a/result/charge_correlation/charge_correlation.xlsx
+++ b/result/charge_correlation/charge_correlation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="53120" yWindow="6560" windowWidth="23320" windowHeight="18840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26900" windowHeight="21080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,45 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Charge of the peptide</t>
+  </si>
+  <si>
+    <t>Hit</t>
+  </si>
+  <si>
+    <t>Not a Hit</t>
+  </si>
+  <si>
+    <t>Estimated Probability of a Hit</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +79,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -67,10 +105,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
+      <c14:style val="119"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="18"/>
+      <c:style val="19"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -97,19 +135,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -143,19 +180,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -189,19 +225,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -235,19 +270,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -281,19 +315,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -327,19 +360,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -373,19 +405,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -419,19 +450,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -465,19 +495,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -511,19 +540,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -557,19 +585,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -603,19 +630,18 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:numRef>
+            <c:strRef>
               <c:f>Sheet1!$A$2:$A$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Not a Hit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -643,11 +669,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2095198792"/>
-        <c:axId val="2095200200"/>
+        <c:axId val="2069228696"/>
+        <c:axId val="2069231944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2095198792"/>
+        <c:axId val="2069228696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -657,7 +683,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095200200"/>
+        <c:crossAx val="2069231944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -665,7 +691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095200200"/>
+        <c:axId val="2069231944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +702,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095198792"/>
+        <c:crossAx val="2069228696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -728,7 +754,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>Hit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -834,7 +860,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>Not a Hit</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -941,11 +967,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2134995240"/>
-        <c:axId val="2143832872"/>
+        <c:axId val="2071326520"/>
+        <c:axId val="2071329496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2134995240"/>
+        <c:axId val="2071326520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -955,7 +981,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143832872"/>
+        <c:crossAx val="2071329496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -963,7 +989,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2143832872"/>
+        <c:axId val="2071329496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,7 +1000,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134995240"/>
+        <c:crossAx val="2071326520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1383,15 +1409,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1">
         <v>-7</v>
       </c>
@@ -1430,7 +1462,7 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
@@ -1471,8 +1503,8 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3">
-        <v>0</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1509,10 +1541,64 @@
       </c>
       <c r="M3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <f>B2/(B2+B3)</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:M4" si="0">C2/(C2+C3)</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7027027027027029E-2</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>8.2644628099173556E-3</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>6.1946902654867256E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.16049382716049382</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.22807017543859648</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>